<commit_message>
UI Validations added V.41
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A4A72B-89A1-45DD-9E85-967E2C45219C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4949B533-6D60-4545-8A33-D94B1C3C2499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,18 +292,12 @@
     <t>100.00 USD</t>
   </si>
   <si>
-    <t>1500.00 USD</t>
-  </si>
-  <si>
     <t>400.00 USD</t>
   </si>
   <si>
     <t>475.00 USD</t>
   </si>
   <si>
-    <t>2000.00 USD</t>
-  </si>
-  <si>
     <t>500.00 USD</t>
   </si>
   <si>
@@ -329,6 +323,12 @@
   </si>
   <si>
     <t>7263709</t>
+  </si>
+  <si>
+    <t>2,000.00 USD</t>
+  </si>
+  <si>
+    <t>1,500.00 USD</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -432,20 +432,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -733,10 +729,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,13 +761,13 @@
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -779,41 +775,41 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3">
         <v>7263707</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3">
         <v>7263708</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>102</v>
+      <c r="D3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="B4" t="s">
         <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -821,13 +817,13 @@
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -835,13 +831,13 @@
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -849,13 +845,13 @@
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -863,13 +859,13 @@
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -877,13 +873,13 @@
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -891,27 +887,27 @@
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>98</v>
+      <c r="B11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>40</v>
       </c>
     </row>
@@ -919,13 +915,13 @@
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -933,13 +929,13 @@
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" t="s">
         <v>42</v>
       </c>
     </row>
@@ -947,13 +943,13 @@
       <c r="A15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -961,13 +957,13 @@
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -975,13 +971,13 @@
       <c r="A17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>49</v>
       </c>
     </row>
@@ -989,13 +985,13 @@
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="5">
         <v>2221</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1003,13 +999,13 @@
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1017,13 +1013,13 @@
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1031,13 +1027,13 @@
       <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1045,27 +1041,27 @@
       <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="B22" t="s">
         <v>95</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1073,13 +1069,13 @@
       <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1087,13 +1083,13 @@
       <c r="A25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1101,13 +1097,13 @@
       <c r="A26" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1115,13 +1111,13 @@
       <c r="A27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1129,69 +1125,69 @@
       <c r="A28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>94</v>
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>90</v>
+      <c r="C29" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>93</v>
+      <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>93</v>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1199,27 +1195,27 @@
       <c r="A33" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="9" t="s">
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>91</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="9" t="s">
+      <c r="B34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1227,13 +1223,13 @@
       <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="9" t="s">
+      <c r="B35" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1241,13 +1237,13 @@
       <c r="A36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="9" t="s">
+      <c r="B36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1255,13 +1251,13 @@
       <c r="A37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="9" t="s">
+      <c r="B37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1269,13 +1265,13 @@
       <c r="A38" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="14" t="s">
+      <c r="B38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="12" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1283,27 +1279,27 @@
       <c r="A39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>90</v>
+      <c r="B39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="9" t="s">
+      <c r="B40" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1311,13 +1307,13 @@
       <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="9" t="s">
+      <c r="B41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1325,13 +1321,13 @@
       <c r="A42" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="14" t="s">
+      <c r="B42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="12" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1339,13 +1335,13 @@
       <c r="A43" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="9" t="s">
+      <c r="B43" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1353,13 +1349,13 @@
       <c r="A44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="9" t="s">
+      <c r="B44" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1367,13 +1363,13 @@
       <c r="A45" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="9" t="s">
+      <c r="B45" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1381,13 +1377,13 @@
       <c r="A46" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="14" t="s">
+      <c r="B46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="12" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1395,13 +1391,13 @@
       <c r="A47" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="9" t="s">
+      <c r="B47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1409,25 +1405,15 @@
       <c r="A48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="9" t="s">
+      <c r="B48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="7"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="7"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="7"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
UI Validations added V.42
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4949B533-6D60-4545-8A33-D94B1C3C2499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157C6B48-0F8A-46AF-A72E-95FBC51FF978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="104">
   <si>
     <t>CountryCode</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>1,500.00 USD</t>
+  </si>
+  <si>
+    <t>1500.00 USD</t>
   </si>
 </sst>
 </file>
@@ -731,8 +734,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1283,10 +1286,10 @@
         <v>51</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
UI Validations added V.44
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157C6B48-0F8A-46AF-A72E-95FBC51FF978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73FD480-D501-484A-8670-F48173CE67DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,7 +735,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
UI Validations added V.65
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54876D23-1958-4AFE-9C95-6BA5BA4EC02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00368758-43E9-49CB-8B47-494F60BFF302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="100">
   <si>
     <t>HeaderCloumnName</t>
   </si>
@@ -94,9 +94,6 @@
     <t>SubmissionDate</t>
   </si>
   <si>
-    <t>10-01-2024</t>
-  </si>
-  <si>
     <t>ArticleTitle</t>
   </si>
   <si>
@@ -166,15 +163,6 @@
     <t>MauScriptId</t>
   </si>
   <si>
-    <t>CAM4-2024-04-7244</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-9832</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-3631</t>
-  </si>
-  <si>
     <t>SubmittedBy</t>
   </si>
   <si>
@@ -208,9 +196,6 @@
     <t>BaseAPCPrice</t>
   </si>
   <si>
-    <t>2,000.00 USD</t>
-  </si>
-  <si>
     <t>BaseArticleTypeDiscount</t>
   </si>
   <si>
@@ -229,12 +214,6 @@
     <t>TotalCharge</t>
   </si>
   <si>
-    <t>1,800.00 USD</t>
-  </si>
-  <si>
-    <t>1,401.20 USD</t>
-  </si>
-  <si>
     <t>DiscountType1</t>
   </si>
   <si>
@@ -271,12 +250,6 @@
     <t>Value1</t>
   </si>
   <si>
-    <t>200.00 USD</t>
-  </si>
-  <si>
-    <t>598.80 USD</t>
-  </si>
-  <si>
     <t>Applied1</t>
   </si>
   <si>
@@ -292,15 +265,9 @@
     <t>Percentage2</t>
   </si>
   <si>
-    <t>0%</t>
-  </si>
-  <si>
     <t>Value2</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>DiscountType3</t>
   </si>
   <si>
@@ -314,6 +281,45 @@
   </si>
   <si>
     <t>Value3</t>
+  </si>
+  <si>
+    <t>10-08-2024</t>
+  </si>
+  <si>
+    <t>CAM4-2024-04-9760</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-4086</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-5225</t>
+  </si>
+  <si>
+    <t>4,700.00 USD</t>
+  </si>
+  <si>
+    <t>1,175.00 USD</t>
+  </si>
+  <si>
+    <t>3,525.00 USD</t>
+  </si>
+  <si>
+    <t>1,800.00 USD::1,057.50 USD</t>
+  </si>
+  <si>
+    <t>823.21 USD</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>3525.00 USD</t>
+  </si>
+  <si>
+    <t>117.50 USD</t>
+  </si>
+  <si>
+    <t>NA::351.80 USD</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -417,20 +423,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -718,10 +720,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -764,29 +766,25 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -794,13 +792,13 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -808,13 +806,13 @@
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -822,13 +820,13 @@
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -836,13 +834,13 @@
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -850,13 +848,13 @@
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -864,679 +862,539 @@
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>24</v>
+      <c r="B11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>26</v>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>28</v>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>30</v>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>32</v>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>35</v>
+      <c r="D16" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>37</v>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="9">
+        <v>37</v>
+      </c>
+      <c r="B18" s="5">
         <v>2221</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>39</v>
+      <c r="C18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>41</v>
+      <c r="C19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>44</v>
+      <c r="D20" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>46</v>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>20</v>
+        <v>71</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>86</v>
+        <v>76</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>88</v>
+        <v>78</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>90</v>
+        <v>80</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>92</v>
+        <v>81</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D44" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>76</v>
+        <v>83</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="7"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="7"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="7"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="7"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B51" s="7"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B52" s="7"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B53" s="7"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B54" s="7"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="7"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B55" s="7"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B56" s="7"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="7"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B57" s="7"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="7"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B58" s="7"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B59" s="7"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="7"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B60" s="7"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="7"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B61" s="7"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="7"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B62" s="7"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="7"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B63" s="7"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="7"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B64" s="7"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B65" s="7"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B66" s="7"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B67" s="7"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="7"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B68" s="7"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="7"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B69" s="7"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B70" s="7"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="7"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B71" s="7"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="7"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B72" s="7"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="7"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B73" s="7"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="7"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B74" s="7"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="7"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B75" s="7"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="7"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B76" s="7"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{F611879D-40B7-449E-8FA9-5AFD0019FD2C}"/>
+    <hyperlink ref="C16" r:id="rId2" xr:uid="{5B93B8B5-E301-4876-8787-30078F6D53FD}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{C0F20163-C887-497B-AD0E-AA104792E2D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UI Validations added V.66
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00368758-43E9-49CB-8B47-494F60BFF302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5CB4CA-3610-4438-8A32-B548A1C32BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,9 +304,6 @@
     <t>3,525.00 USD</t>
   </si>
   <si>
-    <t>1,800.00 USD::1,057.50 USD</t>
-  </si>
-  <si>
     <t>823.21 USD</t>
   </si>
   <si>
@@ -319,7 +316,10 @@
     <t>117.50 USD</t>
   </si>
   <si>
-    <t>NA::351.80 USD</t>
+    <t>1,057.50 USD</t>
+  </si>
+  <si>
+    <t>351.80 USD</t>
   </si>
 </sst>
 </file>
@@ -722,8 +722,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1174,10 +1174,10 @@
         <v>91</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1244,10 +1244,10 @@
         <v>38</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1258,10 +1258,10 @@
         <v>38</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -1314,7 +1314,7 @@
         <v>38</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>99</v>
@@ -1387,7 +1387,7 @@
         <v>38</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.69
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5CB4CA-3610-4438-8A32-B548A1C32BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C2802A-64A6-414A-9FB4-D2390100A555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
   <si>
     <t>HeaderCloumnName</t>
   </si>
@@ -94,6 +94,9 @@
     <t>SubmissionDate</t>
   </si>
   <si>
+    <t>10-15-2024</t>
+  </si>
+  <si>
     <t>ArticleTitle</t>
   </si>
   <si>
@@ -163,6 +166,15 @@
     <t>MauScriptId</t>
   </si>
   <si>
+    <t>CAM4-2024-04-2925</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-4633</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-4422</t>
+  </si>
+  <si>
     <t>SubmittedBy</t>
   </si>
   <si>
@@ -196,6 +208,9 @@
     <t>BaseAPCPrice</t>
   </si>
   <si>
+    <t>4,700.00 USD</t>
+  </si>
+  <si>
     <t>BaseArticleTypeDiscount</t>
   </si>
   <si>
@@ -214,30 +229,33 @@
     <t>TotalCharge</t>
   </si>
   <si>
+    <t>4,230.00 USD</t>
+  </si>
+  <si>
+    <t>3,292.82 USD</t>
+  </si>
+  <si>
+    <t>DiscountType2</t>
+  </si>
+  <si>
     <t>DiscountType1</t>
   </si>
   <si>
     <t>WileyPromoCode</t>
   </si>
   <si>
-    <t>DiscountType2</t>
-  </si>
-  <si>
-    <t>ArticleType</t>
+    <t>DiscountCondition2</t>
+  </si>
+  <si>
+    <t>JCASP</t>
   </si>
   <si>
     <t>DiscountCondition1</t>
   </si>
   <si>
-    <t>JCASP</t>
-  </si>
-  <si>
     <t>PROMO50</t>
   </si>
   <si>
-    <t>DiscountCondition2</t>
-  </si>
-  <si>
     <t>Percentage1</t>
   </si>
   <si>
@@ -250,6 +268,12 @@
     <t>Value1</t>
   </si>
   <si>
+    <t>470.00 USD</t>
+  </si>
+  <si>
+    <t>1407.18 USD</t>
+  </si>
+  <si>
     <t>Applied1</t>
   </si>
   <si>
@@ -281,45 +305,6 @@
   </si>
   <si>
     <t>Value3</t>
-  </si>
-  <si>
-    <t>10-08-2024</t>
-  </si>
-  <si>
-    <t>CAM4-2024-04-9760</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-4086</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-5225</t>
-  </si>
-  <si>
-    <t>4,700.00 USD</t>
-  </si>
-  <si>
-    <t>1,175.00 USD</t>
-  </si>
-  <si>
-    <t>3,525.00 USD</t>
-  </si>
-  <si>
-    <t>823.21 USD</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
-    <t>3525.00 USD</t>
-  </si>
-  <si>
-    <t>117.50 USD</t>
-  </si>
-  <si>
-    <t>1,057.50 USD</t>
-  </si>
-  <si>
-    <t>351.80 USD</t>
   </si>
 </sst>
 </file>
@@ -411,7 +396,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -423,16 +408,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -722,8 +714,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -766,25 +758,29 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -792,13 +788,13 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -806,13 +802,13 @@
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -820,13 +816,13 @@
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -834,13 +830,13 @@
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -848,13 +844,13 @@
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -862,539 +858,539 @@
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>87</v>
+      <c r="B11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
+      <c r="B13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
+      <c r="B15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>34</v>
+      <c r="C16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
+      <c r="B17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="5">
+        <v>38</v>
+      </c>
+      <c r="B18" s="10">
         <v>2221</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>38</v>
+      <c r="C18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>40</v>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>43</v>
+      <c r="C20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
+      <c r="B21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>90</v>
+        <v>47</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
+        <v>51</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>92</v>
+        <v>61</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>93</v>
+        <v>63</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>91</v>
+        <v>65</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>94</v>
+        <v>68</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>65</v>
+      <c r="D35" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>20</v>
+        <v>74</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>95</v>
+        <v>78</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>77</v>
+        <v>84</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>74</v>
+        <v>88</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>73</v>
+        <v>39</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" xr:uid="{F611879D-40B7-449E-8FA9-5AFD0019FD2C}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{5B93B8B5-E301-4876-8787-30078F6D53FD}"/>
-    <hyperlink ref="D16" r:id="rId3" xr:uid="{C0F20163-C887-497B-AD0E-AA104792E2D8}"/>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UI Validations added V.77
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C2802A-64A6-414A-9FB4-D2390100A555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B08880-9D92-4A6A-9C1C-1C384CFE2134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="94">
   <si>
     <t>HeaderCloumnName</t>
   </si>
@@ -49,9 +49,6 @@
     <t>ResponseCode</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>CaseName</t>
   </si>
   <si>
@@ -94,7 +91,7 @@
     <t>SubmissionDate</t>
   </si>
   <si>
-    <t>10-15-2024</t>
+    <t>01-08-2025</t>
   </si>
   <si>
     <t>ArticleTitle</t>
@@ -166,13 +163,13 @@
     <t>MauScriptId</t>
   </si>
   <si>
-    <t>CAM4-2024-04-2925</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-4633</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-4422</t>
+    <t>CAM4-2024-04-3746</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-9254</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-4180</t>
   </si>
   <si>
     <t>SubmittedBy</t>
@@ -232,9 +229,6 @@
     <t>4,230.00 USD</t>
   </si>
   <si>
-    <t>3,292.82 USD</t>
-  </si>
-  <si>
     <t>DiscountType2</t>
   </si>
   <si>
@@ -253,7 +247,7 @@
     <t>DiscountCondition1</t>
   </si>
   <si>
-    <t>PROMO50</t>
+    <t>PCOR</t>
   </si>
   <si>
     <t>Percentage1</t>
@@ -262,7 +256,7 @@
     <t>10%</t>
   </si>
   <si>
-    <t>29.94%</t>
+    <t>100%</t>
   </si>
   <si>
     <t>Value1</t>
@@ -271,7 +265,7 @@
     <t>470.00 USD</t>
   </si>
   <si>
-    <t>1407.18 USD</t>
+    <t>4700.00 USD</t>
   </si>
   <si>
     <t>Applied1</t>
@@ -290,6 +284,9 @@
   </si>
   <si>
     <t>Value2</t>
+  </si>
+  <si>
+    <t>470.00USD</t>
   </si>
   <si>
     <t>DiscountType3</t>
@@ -396,37 +393,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -714,15 +704,15 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.7265625" customWidth="1"/>
-    <col min="3" max="3" width="27" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -733,10 +723,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -758,632 +748,617 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>15</v>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>20</v>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>22</v>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>24</v>
+      <c r="C11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>26</v>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>28</v>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>30</v>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>32</v>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>35</v>
+      <c r="D16" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>37</v>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="10">
+        <v>37</v>
+      </c>
+      <c r="B18" s="6">
         <v>2221</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>39</v>
+      <c r="C18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>41</v>
+      <c r="C19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>44</v>
+      <c r="D20" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>46</v>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>32</v>
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>54</v>
+      <c r="D24" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>54</v>
+      <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>58</v>
+      <c r="C26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>60</v>
+      <c r="C27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>62</v>
+      <c r="C28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>64</v>
+      <c r="C29" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>70</v>
+      <c r="D33" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>39</v>
+        <v>69</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>73</v>
+      <c r="D35" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>39</v>
+        <v>72</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>39</v>
+        <v>87</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>39</v>
+        <v>89</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>39</v>
+        <v>90</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>39</v>
+        <v>91</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>39</v>
+        <v>92</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>39</v>
+        <v>93</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.78
</commit_message>
<xml_diff>
--- a/UploadExcel/TD_PPUIValidations.xlsx
+++ b/UploadExcel/TD_PPUIValidations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B08880-9D92-4A6A-9C1C-1C384CFE2134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A495496-07E8-44F7-A780-33D0179682BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
   <si>
     <t>HeaderCloumnName</t>
   </si>
@@ -284,9 +284,6 @@
   </si>
   <si>
     <t>Value2</t>
-  </si>
-  <si>
-    <t>470.00USD</t>
   </si>
   <si>
     <t>DiscountType3</t>
@@ -704,8 +701,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1288,12 +1285,12 @@
         <v>38</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>38</v>
@@ -1307,7 +1304,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>38</v>
@@ -1321,7 +1318,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>38</v>
@@ -1335,7 +1332,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>38</v>
@@ -1349,7 +1346,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>38</v>

</xml_diff>